<commit_message>
fullfil some client functions and examples
</commit_message>
<xml_diff>
--- a/core/text.xlsx
+++ b/core/text.xlsx
@@ -8,20 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog\Python\ccuoa-client\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4762B49-362B-471C-9064-2BAEE1027B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4276D2B3-057A-4E78-A7A1-2F9BBE43416D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1035" windowWidth="22905" windowHeight="11910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="第n批次德育分申请表（收集结果）" sheetId="1" r:id="rId1"/>
     <sheet name="mapping" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>审核状态</t>
   </si>
@@ -196,6 +207,12 @@
   <si>
     <t>审核时间</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请分数（必填）</t>
+  </si>
+  <si>
+    <t>审核备注</t>
   </si>
 </sst>
 </file>
@@ -569,11 +586,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F38" sqref="F38"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -658,6 +675,76 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -666,10 +753,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A04F8B3-88ED-4FAE-B380-DBB7DD5D7A2E}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="D3" sqref="D3:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -678,12 +765,12 @@
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -694,104 +781,194 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="str">
+        <f>"{'"&amp;A3&amp;"'"&amp;":"&amp;"'"&amp;B3&amp;"'"&amp;"}"&amp;","</f>
+        <v>{'student_id':'学号（必填）'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D14" si="0">"{'"&amp;A4&amp;"'"&amp;":"&amp;"'"&amp;B4&amp;"'"&amp;"}"&amp;","</f>
+        <v>{'student_name':'姓名（必填）'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_types':'申请类型（必填）'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_score':'申请分数（必填）'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_urls':'材料附件（必填）'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_desc':'活动描述（必填）'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_date':'活动时间（必填）'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_msg':'备注'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>{'rec_status':'审核状态'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>{'chk_username':'审核员'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>{'chk_commit':'审核备注'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
       <c r="C14" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>{'chk_date':'审核日期'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>